<commit_message>
mise a jour warping
</commit_message>
<xml_diff>
--- a/GestionProjetSuivi2D.xlsx
+++ b/GestionProjetSuivi2D.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="180" yWindow="0" windowWidth="25600" windowHeight="15880" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
   <si>
     <t>Taches</t>
   </si>
@@ -94,6 +94,30 @@
   </si>
   <si>
     <t>Fabienne&amp;Marion</t>
+  </si>
+  <si>
+    <t>4H30</t>
+  </si>
+  <si>
+    <t>Implémentation du warping</t>
+  </si>
+  <si>
+    <t>4H</t>
+  </si>
+  <si>
+    <t>cahier des charges</t>
+  </si>
+  <si>
+    <t>planing sur MS</t>
+  </si>
+  <si>
+    <t>2H</t>
+  </si>
+  <si>
+    <t>rectifier le warping</t>
+  </si>
+  <si>
+    <t>mettre des commentaires + indentation</t>
   </si>
 </sst>
 </file>
@@ -162,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -170,6 +194,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -606,9 +631,15 @@
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
@@ -620,7 +651,7 @@
       <c r="C8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -634,10 +665,10 @@
       <c r="C9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="4">
         <v>15</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="7">
         <v>42060</v>
       </c>
     </row>
@@ -648,6 +679,89 @@
       <c r="C10" s="5" t="s">
         <v>24</v>
       </c>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="6">
+        <v>42060</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="6">
+        <v>42081</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="6">
+        <v>42081</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="6">
+        <v>42081</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="6">
+        <v>42081</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
a ne pas inclure
</commit_message>
<xml_diff>
--- a/GestionProjetSuivi2D.xlsx
+++ b/GestionProjetSuivi2D.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
   <si>
     <t>Taches</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Calcul  de l’erreur</t>
   </si>
   <si>
-    <t>méthode permettant de remettre l’image dans la bonne zone</t>
-  </si>
-  <si>
     <t>Mise à jour du vecteur a</t>
   </si>
   <si>
@@ -85,9 +82,6 @@
   </si>
   <si>
     <t xml:space="preserve">Tracking : regarder les méthodes </t>
-  </si>
-  <si>
-    <t>Bene</t>
   </si>
   <si>
     <t>1H30</t>
@@ -526,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -554,7 +548,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -562,12 +556,14 @@
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="E2" s="6">
         <v>42053</v>
       </c>
@@ -577,12 +573,14 @@
         <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="E3" s="6">
         <v>42053</v>
       </c>
@@ -592,12 +590,14 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="4"/>
+        <v>12</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="E4" s="6">
         <v>42053</v>
       </c>
@@ -607,13 +607,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" s="6">
         <v>42060</v>
@@ -623,36 +623,45 @@
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="C7" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>23</v>
+        <v>12</v>
+      </c>
+      <c r="D8" s="4">
+        <v>15</v>
+      </c>
+      <c r="E8" s="7">
+        <v>42060</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -660,50 +669,56 @@
         <v>20</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="4">
-        <v>15</v>
-      </c>
-      <c r="E9" s="7">
+        <v>22</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="6">
         <v>42060</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="6">
+        <v>42060</v>
+      </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>25</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="D11" s="4"/>
       <c r="E11" s="6">
-        <v>42060</v>
+        <v>42081</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>12</v>
@@ -715,53 +730,46 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="E13" s="6">
         <v>42081</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="4"/>
+      <c r="D14" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="E14" s="6">
         <v>42081</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="6">
-        <v>42081</v>
-      </c>
+      <c r="A15" s="2"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="2"/>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>